<commit_message>
Updated test cases report with JWT Token failures
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111MEDIACLINICS/MEDIACLINICS_ITALIA/V.3.3.0/accreditamento-MEDIACLINICS_ITALIA-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111MEDIACLINICS/MEDIACLINICS_ITALIA/V.3.3.0/accreditamento-MEDIACLINICS_ITALIA-checklist_V4.1.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -272,6 +272,9 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
+    <t>NO</t>
+  </si>
+  <si>
     <t>Campi opzionali non gestiti da applicativo.</t>
   </si>
   <si>
@@ -317,6 +320,18 @@
       <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.</t>
     </r>
+  </si>
+  <si>
+    <t>24/02/2023</t>
+  </si>
+  <si>
+    <t>2023-02-24T09:23:18.4740079+01:00</t>
+  </si>
+  <si>
+    <t>7261b3b75e747926</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
     <t>Viene segnalato all'operatore un errore con il Gateway e si richiede di provare più tardi.</t>
@@ -367,6 +382,12 @@
     </r>
   </si>
   <si>
+    <t>2023-02-16T17:11:16.1164403+01:00</t>
+  </si>
+  <si>
+    <t>7ade263185140c8f</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_LDO_TIMEOUT</t>
   </si>
   <si>
@@ -383,12 +404,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
-  </si>
-  <si>
-    <t>2023-02-16T17:11:16.1164403+01:00</t>
-  </si>
-  <si>
-    <t>7ade263185140c8f</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.1.1.1dd306de0de59f6790e5c6d343934d3682f111a52a98e148274074dcffdf2877.5c6e9df112^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
@@ -569,9 +584,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>Campi ozpionali non gestiti da applicativo.</t>
-  </si>
-  <si>
     <t>ID TEST CASE OK</t>
   </si>
   <si>
@@ -637,15 +649,12 @@
   <si>
     <t>FAIL</t>
   </si>
-  <si>
-    <t>NO</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -674,6 +683,11 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
@@ -988,7 +1002,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="70">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1096,17 +1110,39 @@
     <xf borderId="16" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="15" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="16" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="17" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="17" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="17" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="17" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="18" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1141,7 +1177,7 @@
     <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2519,7 +2555,7 @@
     <col customWidth="1" min="10" max="10" width="45.43"/>
     <col customWidth="1" min="11" max="11" width="27.29"/>
     <col customWidth="1" min="12" max="12" width="20.14"/>
-    <col customWidth="1" min="13" max="13" width="21.71"/>
+    <col customWidth="1" min="13" max="13" width="40.43"/>
     <col customWidth="1" min="14" max="14" width="22.0"/>
     <col customWidth="1" min="15" max="15" width="31.71"/>
     <col customWidth="1" min="16" max="26" width="8.71"/>
@@ -2834,79 +2870,119 @@
       <c r="H13" s="32"/>
       <c r="I13" s="33"/>
       <c r="J13" s="34"/>
-      <c r="K13" s="36"/>
+      <c r="K13" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="42" t="s">
-        <v>50</v>
-      </c>
+      <c r="M13" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="42"/>
+      <c r="O13" s="41"/>
     </row>
     <row r="14" ht="183.75" customHeight="1">
-      <c r="A14" s="28">
+      <c r="A14" s="43">
         <v>29.0</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="30" t="s">
+      <c r="D14" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
+      <c r="E14" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>57</v>
+      </c>
       <c r="J14" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="41" t="s">
+      <c r="L14" s="47"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="O14" s="38"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="51"/>
     </row>
     <row r="15" ht="183.75" customHeight="1">
-      <c r="A15" s="28">
+      <c r="A15" s="43">
         <v>37.0</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33"/>
+      <c r="G15" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>57</v>
+      </c>
       <c r="J15" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="35"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="41" t="s">
+      <c r="L15" s="47"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="38"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="51"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
+      <c r="Y15" s="51"/>
+      <c r="Z15" s="51"/>
     </row>
     <row r="16" ht="65.25" customHeight="1">
       <c r="A16" s="28">
@@ -2919,24 +2995,24 @@
         <v>30</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F16" s="40"/>
       <c r="G16" s="32"/>
       <c r="H16" s="32"/>
       <c r="I16" s="33"/>
-      <c r="J16" s="43" t="s">
-        <v>58</v>
+      <c r="J16" s="52" t="s">
+        <v>65</v>
       </c>
       <c r="K16" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L16" s="35"/>
       <c r="M16" s="36"/>
-      <c r="N16" s="41" t="s">
+      <c r="N16" s="42" t="s">
         <v>37</v>
       </c>
       <c r="O16" s="38"/>
@@ -2952,10 +3028,10 @@
         <v>30</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F17" s="31" t="s">
         <v>33</v>
@@ -2967,21 +3043,21 @@
         <v>62</v>
       </c>
       <c r="I17" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="43" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="J17" s="52" t="s">
+        <v>69</v>
       </c>
       <c r="K17" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L17" s="35"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="41" t="s">
+      <c r="M17" s="35"/>
+      <c r="N17" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="42" t="s">
-        <v>65</v>
+      <c r="O17" s="41" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="18" ht="72.0" customHeight="1">
@@ -2995,32 +3071,32 @@
         <v>30</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="I18" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="J18" s="43" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="J18" s="52" t="s">
+        <v>76</v>
       </c>
       <c r="K18" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L18" s="35"/>
       <c r="M18" s="36"/>
-      <c r="N18" s="41" t="s">
+      <c r="N18" s="42" t="s">
         <v>37</v>
       </c>
       <c r="O18" s="38"/>
@@ -3036,32 +3112,32 @@
         <v>30</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I19" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" s="52" t="s">
         <v>76</v>
-      </c>
-      <c r="J19" s="43" t="s">
-        <v>71</v>
       </c>
       <c r="K19" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L19" s="35"/>
       <c r="M19" s="36"/>
-      <c r="N19" s="41" t="s">
+      <c r="N19" s="42" t="s">
         <v>37</v>
       </c>
       <c r="O19" s="38"/>
@@ -3077,32 +3153,32 @@
         <v>30</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H20" s="32" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I20" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="J20" s="43" t="s">
-        <v>71</v>
+        <v>86</v>
+      </c>
+      <c r="J20" s="52" t="s">
+        <v>76</v>
       </c>
       <c r="K20" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L20" s="35"/>
       <c r="M20" s="36"/>
-      <c r="N20" s="41" t="s">
+      <c r="N20" s="42" t="s">
         <v>37</v>
       </c>
       <c r="O20" s="38"/>
@@ -3118,32 +3194,32 @@
         <v>30</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F21" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I21" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="J21" s="43" t="s">
-        <v>71</v>
+        <v>91</v>
+      </c>
+      <c r="J21" s="52" t="s">
+        <v>76</v>
       </c>
       <c r="K21" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L21" s="35"/>
       <c r="M21" s="36"/>
-      <c r="N21" s="41" t="s">
+      <c r="N21" s="42" t="s">
         <v>37</v>
       </c>
       <c r="O21" s="38"/>
@@ -3159,36 +3235,36 @@
         <v>30</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F22" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="I22" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="J22" s="43" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+      <c r="J22" s="52" t="s">
+        <v>97</v>
       </c>
       <c r="K22" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L22" s="35"/>
       <c r="M22" s="36"/>
-      <c r="N22" s="41" t="s">
+      <c r="N22" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="O22" s="42" t="s">
-        <v>93</v>
+      <c r="O22" s="41" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="23" ht="72.0" customHeight="1">
@@ -3202,32 +3278,32 @@
         <v>30</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="I23" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="J23" s="43" t="s">
-        <v>71</v>
+        <v>103</v>
+      </c>
+      <c r="J23" s="52" t="s">
+        <v>76</v>
       </c>
       <c r="K23" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L23" s="35"/>
       <c r="M23" s="36"/>
-      <c r="N23" s="41" t="s">
+      <c r="N23" s="42" t="s">
         <v>37</v>
       </c>
       <c r="O23" s="38"/>
@@ -3243,32 +3319,32 @@
         <v>30</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I24" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="J24" s="43" t="s">
-        <v>71</v>
+        <v>108</v>
+      </c>
+      <c r="J24" s="52" t="s">
+        <v>76</v>
       </c>
       <c r="K24" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L24" s="35"/>
       <c r="M24" s="36"/>
-      <c r="N24" s="41" t="s">
+      <c r="N24" s="42" t="s">
         <v>37</v>
       </c>
       <c r="O24" s="38"/>
@@ -3284,23 +3360,25 @@
         <v>30</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F25" s="40"/>
       <c r="G25" s="32"/>
       <c r="H25" s="32"/>
       <c r="I25" s="33"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="36"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="42" t="s">
-        <v>50</v>
-      </c>
+      <c r="M25" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="N25" s="42"/>
+      <c r="O25" s="41"/>
     </row>
     <row r="26" ht="72.0" customHeight="1">
       <c r="A26" s="28">
@@ -3313,23 +3391,25 @@
         <v>30</v>
       </c>
       <c r="D26" s="44" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F26" s="40"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
       <c r="I26" s="33"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="36"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="42" t="s">
-        <v>50</v>
-      </c>
+      <c r="M26" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="N26" s="42"/>
+      <c r="O26" s="41"/>
     </row>
     <row r="27" ht="72.0" customHeight="1">
       <c r="A27" s="28">
@@ -3342,32 +3422,32 @@
         <v>30</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H27" s="32" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="I27" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="J27" s="43" t="s">
-        <v>64</v>
+        <v>117</v>
+      </c>
+      <c r="J27" s="52" t="s">
+        <v>69</v>
       </c>
       <c r="K27" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L27" s="35"/>
       <c r="M27" s="36"/>
-      <c r="N27" s="41" t="s">
+      <c r="N27" s="42" t="s">
         <v>37</v>
       </c>
       <c r="O27" s="38"/>
@@ -3383,23 +3463,25 @@
         <v>30</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="32"/>
       <c r="H28" s="32"/>
       <c r="I28" s="33"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="36"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="42" t="s">
-        <v>115</v>
-      </c>
+      <c r="M28" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="N28" s="42"/>
+      <c r="O28" s="41"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="F29" s="7"/>
@@ -13589,101 +13671,101 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="48" t="s">
-        <v>117</v>
+      <c r="C1" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>121</v>
+      <c r="A2" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="52" t="s">
+      <c r="B3" s="62" t="s">
         <v>123</v>
       </c>
+      <c r="C3" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="53" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="55" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="56" t="s">
-        <v>126</v>
+      <c r="A4" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="64" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="55" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>129</v>
+      <c r="A5" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="56" t="s">
-        <v>132</v>
+      <c r="A6" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="57" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>135</v>
+      <c r="A7" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1"/>
@@ -14701,27 +14783,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="68" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="60" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="60" t="s">
+      <c r="A2" s="68" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="61" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>138</v>
+      <c r="A3" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Fixed excel report file problems
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111MEDIACLINICS/MEDIACLINICS_ITALIA/V.3.3.0/accreditamento-MEDIACLINICS_ITALIA-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111MEDIACLINICS/MEDIACLINICS_ITALIA/V.3.3.0/accreditamento-MEDIACLINICS_ITALIA-checklist_V4.1.xlsx
@@ -14,7 +14,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mhzpGvxMPjNBWRNRNKekMH6ZXUsPw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mjGP6TuHyHdUhXzKq623Mn5lxS+PA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -53,14 +53,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhY63U84Z84Jg1U+JvtcLKqh7TT6g=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhJ8B56h1DLDxH9ScjA63oZ43WkAQ=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="142">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -654,7 +654,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -683,11 +683,6 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
@@ -1002,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="66">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1040,14 +1035,14 @@
     </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="7" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1084,22 +1079,19 @@
       <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="16" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf borderId="16" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="16" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -1109,12 +1101,6 @@
     </xf>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1129,9 +1115,6 @@
       <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="17" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="17" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="17" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1142,10 +1125,10 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="17" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1177,7 +1160,7 @@
     <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2771,9 +2754,9 @@
         <v>37</v>
       </c>
       <c r="L10" s="35"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="38"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="37"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="28">
@@ -2808,9 +2791,9 @@
         <v>37</v>
       </c>
       <c r="L11" s="35"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="38"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="37"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="28">
@@ -2845,9 +2828,9 @@
         <v>37</v>
       </c>
       <c r="L12" s="35"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="38"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="37"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="28">
@@ -2859,13 +2842,13 @@
       <c r="C13" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="38" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="40"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
       <c r="I13" s="33"/>
@@ -2873,30 +2856,30 @@
       <c r="K13" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="36"/>
-      <c r="M13" s="41" t="s">
+      <c r="L13" s="35"/>
+      <c r="M13" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="N13" s="42"/>
-      <c r="O13" s="41"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="37"/>
     </row>
     <row r="14" ht="183.75" customHeight="1">
-      <c r="A14" s="43">
+      <c r="A14" s="40">
         <v>29.0</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F14" s="43" t="s">
         <v>54</v>
       </c>
       <c r="G14" s="32" t="s">
@@ -2911,44 +2894,44 @@
       <c r="J14" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="47" t="s">
+      <c r="K14" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="47"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="49" t="s">
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="O14" s="50"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
-      <c r="W14" s="51"/>
-      <c r="X14" s="51"/>
-      <c r="Y14" s="51"/>
-      <c r="Z14" s="51"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="47"/>
+      <c r="V14" s="47"/>
+      <c r="W14" s="47"/>
+      <c r="X14" s="47"/>
+      <c r="Y14" s="47"/>
+      <c r="Z14" s="47"/>
     </row>
     <row r="15" ht="183.75" customHeight="1">
-      <c r="A15" s="43">
+      <c r="A15" s="40">
         <v>37.0</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="43" t="s">
         <v>54</v>
       </c>
       <c r="G15" s="32" t="s">
@@ -2963,26 +2946,26 @@
       <c r="J15" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="K15" s="47" t="s">
+      <c r="K15" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="47"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="49" t="s">
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="50"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="51"/>
-      <c r="T15" s="51"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="51"/>
-      <c r="Y15" s="51"/>
-      <c r="Z15" s="51"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="47"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="47"/>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="47"/>
     </row>
     <row r="16" ht="65.25" customHeight="1">
       <c r="A16" s="28">
@@ -3000,22 +2983,22 @@
       <c r="E16" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="40"/>
+      <c r="F16" s="39"/>
       <c r="G16" s="32"/>
       <c r="H16" s="32"/>
       <c r="I16" s="33"/>
-      <c r="J16" s="52" t="s">
+      <c r="J16" s="48" t="s">
         <v>65</v>
       </c>
       <c r="K16" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L16" s="35"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="42" t="s">
+      <c r="M16" s="35"/>
+      <c r="N16" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O16" s="38"/>
+      <c r="O16" s="37"/>
     </row>
     <row r="17" ht="72.0" customHeight="1">
       <c r="A17" s="28">
@@ -3045,7 +3028,7 @@
       <c r="I17" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="J17" s="52" t="s">
+      <c r="J17" s="48" t="s">
         <v>69</v>
       </c>
       <c r="K17" s="35" t="s">
@@ -3053,10 +3036,10 @@
       </c>
       <c r="L17" s="35"/>
       <c r="M17" s="35"/>
-      <c r="N17" s="42" t="s">
+      <c r="N17" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="41" t="s">
+      <c r="O17" s="37" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3088,18 +3071,18 @@
       <c r="I18" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="J18" s="52" t="s">
+      <c r="J18" s="48" t="s">
         <v>76</v>
       </c>
       <c r="K18" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="42" t="s">
+      <c r="M18" s="35"/>
+      <c r="N18" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O18" s="38"/>
+      <c r="O18" s="37"/>
     </row>
     <row r="19" ht="72.0" customHeight="1">
       <c r="A19" s="28">
@@ -3129,18 +3112,18 @@
       <c r="I19" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="J19" s="52" t="s">
+      <c r="J19" s="48" t="s">
         <v>76</v>
       </c>
       <c r="K19" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L19" s="35"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="42" t="s">
+      <c r="M19" s="35"/>
+      <c r="N19" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O19" s="38"/>
+      <c r="O19" s="37"/>
     </row>
     <row r="20" ht="72.0" customHeight="1">
       <c r="A20" s="28">
@@ -3170,18 +3153,18 @@
       <c r="I20" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="J20" s="52" t="s">
+      <c r="J20" s="48" t="s">
         <v>76</v>
       </c>
       <c r="K20" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L20" s="35"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="42" t="s">
+      <c r="M20" s="35"/>
+      <c r="N20" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O20" s="38"/>
+      <c r="O20" s="37"/>
     </row>
     <row r="21" ht="72.0" customHeight="1">
       <c r="A21" s="28">
@@ -3211,18 +3194,18 @@
       <c r="I21" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="J21" s="52" t="s">
+      <c r="J21" s="48" t="s">
         <v>76</v>
       </c>
       <c r="K21" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L21" s="35"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="42" t="s">
+      <c r="M21" s="35"/>
+      <c r="N21" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O21" s="38"/>
+      <c r="O21" s="37"/>
     </row>
     <row r="22" ht="72.0" customHeight="1">
       <c r="A22" s="28">
@@ -3252,18 +3235,18 @@
       <c r="I22" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="J22" s="52" t="s">
+      <c r="J22" s="48" t="s">
         <v>97</v>
       </c>
       <c r="K22" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L22" s="35"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="42" t="s">
+      <c r="M22" s="35"/>
+      <c r="N22" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O22" s="41" t="s">
+      <c r="O22" s="37" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3295,18 +3278,18 @@
       <c r="I23" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="J23" s="52" t="s">
+      <c r="J23" s="48" t="s">
         <v>76</v>
       </c>
       <c r="K23" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L23" s="35"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="42" t="s">
+      <c r="M23" s="35"/>
+      <c r="N23" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O23" s="38"/>
+      <c r="O23" s="37"/>
     </row>
     <row r="24" ht="72.0" customHeight="1">
       <c r="A24" s="28">
@@ -3336,18 +3319,18 @@
       <c r="I24" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="J24" s="52" t="s">
+      <c r="J24" s="48" t="s">
         <v>76</v>
       </c>
       <c r="K24" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L24" s="35"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="42" t="s">
+      <c r="M24" s="35"/>
+      <c r="N24" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O24" s="38"/>
+      <c r="O24" s="37"/>
     </row>
     <row r="25" ht="72.0" customHeight="1">
       <c r="A25" s="28">
@@ -3359,26 +3342,28 @@
       <c r="C25" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="41" t="s">
         <v>109</v>
       </c>
       <c r="E25" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="F25" s="40"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="32"/>
       <c r="H25" s="32"/>
       <c r="I25" s="33"/>
-      <c r="J25" s="53"/>
+      <c r="J25" s="48"/>
       <c r="K25" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="L25" s="36"/>
-      <c r="M25" s="41" t="s">
+      <c r="L25" s="35"/>
+      <c r="M25" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="N25" s="42"/>
-      <c r="O25" s="41"/>
+      <c r="N25" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="37"/>
     </row>
     <row r="26" ht="72.0" customHeight="1">
       <c r="A26" s="28">
@@ -3390,26 +3375,28 @@
       <c r="C26" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="41" t="s">
         <v>111</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="F26" s="40"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
       <c r="I26" s="33"/>
-      <c r="J26" s="53"/>
+      <c r="J26" s="48"/>
       <c r="K26" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="L26" s="36"/>
-      <c r="M26" s="41" t="s">
+      <c r="L26" s="35"/>
+      <c r="M26" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="N26" s="42"/>
-      <c r="O26" s="41"/>
+      <c r="N26" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" s="37"/>
     </row>
     <row r="27" ht="72.0" customHeight="1">
       <c r="A27" s="28">
@@ -3439,18 +3426,18 @@
       <c r="I27" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="J27" s="52" t="s">
+      <c r="J27" s="48" t="s">
         <v>69</v>
       </c>
       <c r="K27" s="35" t="s">
         <v>37</v>
       </c>
       <c r="L27" s="35"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="42" t="s">
+      <c r="M27" s="35"/>
+      <c r="N27" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="O27" s="38"/>
+      <c r="O27" s="37"/>
     </row>
     <row r="28" ht="72.0" customHeight="1">
       <c r="A28" s="28">
@@ -3462,26 +3449,28 @@
       <c r="C28" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="41" t="s">
         <v>118</v>
       </c>
       <c r="E28" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="F28" s="40"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="32"/>
       <c r="H28" s="32"/>
       <c r="I28" s="33"/>
-      <c r="J28" s="53"/>
+      <c r="J28" s="48"/>
       <c r="K28" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="L28" s="36"/>
-      <c r="M28" s="41" t="s">
+      <c r="L28" s="35"/>
+      <c r="M28" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="N28" s="42"/>
-      <c r="O28" s="41"/>
+      <c r="N28" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="O28" s="37"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="F29" s="7"/>
@@ -13671,100 +13660,100 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="52" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="53" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="56" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="56" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="60" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="56" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="60" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="60" t="s">
         <v>139</v>
       </c>
     </row>
@@ -14783,26 +14772,26 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="64" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="64" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="64" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>